<commit_message>
UPDATE added more mapping details to technical mapping file
</commit_message>
<xml_diff>
--- a/zugferd/technical/ZUGFeRD-Mapping.xlsx
+++ b/zugferd/technical/ZUGFeRD-Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17520"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17600"/>
   </bookViews>
   <sheets>
     <sheet name="ebInterface-to-ZUGFeRD" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="166">
   <si>
     <t>Bezeichung in ZUGFeRD</t>
   </si>
@@ -415,6 +415,108 @@
   </si>
   <si>
     <t>todo</t>
+  </si>
+  <si>
+    <t>/Invoice/RelatedDocument</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/DeliveryID</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Period/FromDate</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Period/ToDate</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/AddressIdentifier</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/AddressIdentifier/@AddressIdentifierType</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/Salutation</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/Name</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/Street</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/POBox</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/Town</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/ZIP</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/Country</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/Country/@CountryCode</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/Phone</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/Email</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/Contact</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Address/AddressExtension</t>
+  </si>
+  <si>
+    <t>/Invoice/Delivery/Description</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:ActualDeliverySupplyChainEvent/ram:OccurrenceDateTime/udt:DateTimeString</t>
+  </si>
+  <si>
+    <t>Bedeutung in ebInterface</t>
+  </si>
+  <si>
+    <t>Das Lieferdatum.</t>
+  </si>
+  <si>
+    <t>Lieferperiode von</t>
+  </si>
+  <si>
+    <t>Lieferperiode bis</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:ShipFromTradeParty/ram:DefinedTradeContact/ram:PersonName</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:ShipFromTradeParty/ram:PostalTradeAddress/ram:LineOne</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:ShipFromTradeParty/ram:PostalTradeAddress/ram:CityName</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:ShipFromTradeParty/ram:PostalTradeAddress/ram:PostcodeCode</t>
+  </si>
+  <si>
+    <t>not mapped, since we only consider the country code</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:ShipFromTradeParty/ram:PostalTradeAddress/ram:CountryID</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:ShipFromTradeParty/ram:DefinedTradeContact/ram:TelephoneUniversalCommunication</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:ShipFromTradeParty/ram:DefinedTradeContact/ram:EmailURIUniversalCommunication/ram:CompleteNumber</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:ShipFromTradeParty/ram:Name</t>
+  </si>
+  <si>
+    <t>rsm:CrossIndustryDocument/rsm:SpecifiedSupplyChainTradeTransaction/ram:ApplicableSupplyChainTradeDelivery/ram:DespatchAdviceReferencedDocument/ram:ID</t>
   </si>
 </sst>
 </file>
@@ -484,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -492,8 +594,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
@@ -515,8 +632,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -524,21 +651,34 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -547,11 +687,57 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Result" xfId="3"/>
     <cellStyle name="Result2" xfId="4"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -819,7 +1005,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -827,843 +1013,1280 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="66.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.625" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="2" max="2" width="30.375" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="66.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" ht="30">
+      <c r="A4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E9" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E10" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E11" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30">
-      <c r="A17" s="1" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45">
+      <c r="A15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30">
+      <c r="A20" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="A24" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30">
+      <c r="A27" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45">
+      <c r="A28" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45">
+      <c r="A29" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B49" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C49" s="5"/>
+      <c r="D49" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30">
-      <c r="A18" s="1" t="s">
+      <c r="E49" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30">
+      <c r="A50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B50" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C50" s="5"/>
+      <c r="D50" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30">
-      <c r="A19" s="1" t="s">
+      <c r="E50" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30">
+      <c r="A51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B51" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C51" s="5"/>
+      <c r="D51" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30">
-      <c r="A20" s="1" t="s">
+      <c r="E51" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30">
+      <c r="A52" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B52" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C52" s="5"/>
+      <c r="D52" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30">
-      <c r="A21" s="1" t="s">
+      <c r="E52" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30">
+      <c r="A53" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B53" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C53" s="5"/>
+      <c r="D53" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30">
-      <c r="A22" s="1" t="s">
+      <c r="E53" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30">
+      <c r="A54" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B54" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C54" s="5"/>
+      <c r="D54" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30">
-      <c r="A23" s="1" t="s">
+      <c r="E54" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30">
+      <c r="A55" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B55" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C55" s="5"/>
+      <c r="D55" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D23" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30">
-      <c r="A24" s="1" t="s">
+      <c r="E55" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30">
+      <c r="A56" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B56" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C56" s="5"/>
+      <c r="D56" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30">
-      <c r="A25" s="1" t="s">
+      <c r="E56" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="30">
+      <c r="A57" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B57" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C57" s="5"/>
+      <c r="D57" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D25" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30">
-      <c r="A26" s="1" t="s">
+      <c r="E57" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30">
+      <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B58" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C58" s="5"/>
+      <c r="D58" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D26" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30">
-      <c r="A27" s="1" t="s">
+      <c r="E58" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30">
+      <c r="A59" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B59" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C59" s="5"/>
+      <c r="D59" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30">
-      <c r="A28" s="1" t="s">
+      <c r="E59" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B60" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C60" s="5"/>
+      <c r="D60" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30">
-      <c r="A29" s="1" t="s">
+      <c r="E60" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30">
+      <c r="A61" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B61" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C61" s="5"/>
+      <c r="D61" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30">
-      <c r="A30" s="1" t="s">
+      <c r="E61" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B62" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C62" s="5"/>
+      <c r="D62" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30">
-      <c r="A31" s="1" t="s">
+      <c r="E62" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30">
+      <c r="A63" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B63" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C63" s="5"/>
+      <c r="D63" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30">
-      <c r="A32" s="1" t="s">
+      <c r="E63" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="30">
+      <c r="A64" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B64" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C64" s="5"/>
+      <c r="D64" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30">
-      <c r="A33" s="1" t="s">
+      <c r="E64" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30">
+      <c r="A65" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B65" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C65" s="5"/>
+      <c r="D65" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D33" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30">
-      <c r="A34" s="1" t="s">
+      <c r="E65" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30">
+      <c r="A66" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B66" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C66" s="5"/>
+      <c r="D66" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30">
-      <c r="A35" s="1" t="s">
+      <c r="E66" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="30">
+      <c r="A67" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B67" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C67" s="5"/>
+      <c r="D67" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30">
-      <c r="A36" s="1" t="s">
+      <c r="E67" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30">
+      <c r="A68" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B68" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C68" s="5"/>
+      <c r="D68" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D36" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="30">
-      <c r="A37" s="1" t="s">
+      <c r="E68" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="30">
+      <c r="A69" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B69" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C69" s="5"/>
+      <c r="D69" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D37" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30">
-      <c r="A38" s="1" t="s">
+      <c r="E69" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="30">
+      <c r="A70" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B70" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C70" s="5"/>
+      <c r="D70" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30">
-      <c r="A39" s="1" t="s">
+      <c r="E70" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30">
+      <c r="A71" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B71" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C71" s="5"/>
+      <c r="D71" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D39" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30">
-      <c r="A40" s="1" t="s">
+      <c r="E71" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30">
+      <c r="A72" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B72" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C72" s="5"/>
+      <c r="D72" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D40" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30">
-      <c r="A41" s="1" t="s">
+      <c r="E72" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30">
+      <c r="A73" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B73" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C73" s="5"/>
+      <c r="D73" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D41" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45">
-      <c r="A42" s="1" t="s">
+      <c r="E73" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="45">
+      <c r="A74" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B74" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C74" s="5"/>
+      <c r="D74" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D42" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="30">
-      <c r="A43" s="1" t="s">
+      <c r="E74" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30">
+      <c r="A75" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B75" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C75" s="5"/>
+      <c r="D75" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D43" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30">
-      <c r="A44" s="1" t="s">
+      <c r="E75" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30">
+      <c r="A76" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B76" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C76" s="5"/>
+      <c r="D76" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D44" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30">
-      <c r="A45" s="1" t="s">
+      <c r="E76" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30">
+      <c r="A77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B77" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C77" s="5"/>
+      <c r="D77" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D45" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30">
-      <c r="A46" s="1" t="s">
+      <c r="E77" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30">
+      <c r="A78" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B78" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C78" s="5"/>
+      <c r="D78" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D46" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="30">
-      <c r="A47" s="1" t="s">
+      <c r="E78" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30">
+      <c r="A79" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B79" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C79" s="5"/>
+      <c r="D79" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D47" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="30">
-      <c r="A48" s="1" t="s">
+      <c r="E79" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="30">
+      <c r="A80" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B80" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C80" s="5"/>
+      <c r="D80" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D48" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="30">
-      <c r="A49" s="1" t="s">
+      <c r="E80" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="30">
+      <c r="A81" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B81" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C81" s="5"/>
+      <c r="D81" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D49" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30">
-      <c r="A50" s="1" t="s">
+      <c r="E81" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30">
+      <c r="A82" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B82" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C82" s="5"/>
+      <c r="D82" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D50" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30">
-      <c r="A51" s="1" t="s">
+      <c r="E82" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30">
+      <c r="A83" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B83" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C83" s="5"/>
+      <c r="D83" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D51" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30">
-      <c r="A52" s="1" t="s">
+      <c r="E83" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30">
+      <c r="A84" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B84" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C84" s="5"/>
+      <c r="D84" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D52" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30">
-      <c r="A53" s="1" t="s">
+      <c r="E84" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30">
+      <c r="A85" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B85" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C85" s="5"/>
+      <c r="D85" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D53" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="30">
-      <c r="A54" s="1" t="s">
+      <c r="E85" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30">
+      <c r="A86" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B86" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C86" s="5"/>
+      <c r="D86" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D54" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30">
-      <c r="A55" s="1" t="s">
+      <c r="E86" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30">
+      <c r="A87" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B87" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C87" s="5"/>
+      <c r="D87" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D55" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="30">
-      <c r="A56" s="1" t="s">
+      <c r="E87" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="30">
+      <c r="A88" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B88" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C88" s="5"/>
+      <c r="D88" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D56" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="45">
-      <c r="A57" s="1" t="s">
+      <c r="E88" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="45">
+      <c r="A89" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B89" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C89" s="5"/>
+      <c r="D89" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D57" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="1" t="s">
+      <c r="E89" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="30">
+      <c r="A90" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B90" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C90" s="5"/>
+      <c r="D90" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D58" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="45">
-      <c r="A59" s="1" t="s">
+      <c r="E90" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="45">
+      <c r="A91" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B91" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C91" s="5"/>
+      <c r="D91" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D59" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="30">
-      <c r="A60" s="1" t="s">
+      <c r="E91" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="30">
+      <c r="A92" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B92" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C92" s="5"/>
+      <c r="D92" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D60" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="30">
-      <c r="A61" s="1" t="s">
+      <c r="E92" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="30">
+      <c r="A93" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B93" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C93" s="5"/>
+      <c r="D93" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D61" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30">
-      <c r="A62" s="1" t="s">
+      <c r="E93" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="30">
+      <c r="A94" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B94" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C94" s="5"/>
+      <c r="D94" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D62" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="30">
-      <c r="A63" s="1" t="s">
+      <c r="E94" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="30">
+      <c r="A95" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B95" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C95" s="5"/>
+      <c r="D95" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D63" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="30">
-      <c r="A64" s="1" t="s">
+      <c r="E95" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="30">
+      <c r="A96" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B96" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C96" s="5"/>
+      <c r="D96" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E96" s="5" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="iconSet" priority="1">
+  <conditionalFormatting sqref="A10">
+    <cfRule type="iconSet" priority="3">
       <iconSet iconSet="4Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -1671,12 +2294,20 @@
         <cfvo type="percent" val="75"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
         <cfvo type="percent" val="67"/>
       </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0.4" bottom="0.4" header="0" footer="0"/>

</xml_diff>